<commit_message>
feat(sdm_study): v1.3.0 Engine properly matches transcript x curriculum. Adds new tab_results2 with layout
</commit_message>
<xml_diff>
--- a/T1-Software-Development-Management/projects/TTrack_v1/data/sample_academic_transcript.xlsx
+++ b/T1-Software-Development-Management/projects/TTrack_v1/data/sample_academic_transcript.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Year</t>
   </si>
@@ -37,10 +37,10 @@
     <t>University</t>
   </si>
   <si>
-    <t>SE101</t>
-  </si>
-  <si>
-    <t>Software Engineering Fundamentas</t>
+    <t>SEP401</t>
+  </si>
+  <si>
+    <t>Software Engineering Principles</t>
   </si>
   <si>
     <t>Distinction</t>
@@ -52,32 +52,35 @@
     <t>Torrens</t>
   </si>
   <si>
-    <t>AI201</t>
-  </si>
-  <si>
-    <t>Introduction to Machine Learning</t>
+    <t>SDM404</t>
+  </si>
+  <si>
+    <t>Software Development Management</t>
   </si>
   <si>
     <t>Credit</t>
   </si>
   <si>
-    <t>SE203</t>
-  </si>
-  <si>
-    <t>Data Structures and Algorithms I</t>
+    <t>REM502</t>
+  </si>
+  <si>
+    <t>Research Methodologies</t>
   </si>
   <si>
     <t>High Distinction</t>
   </si>
   <si>
-    <t>Data Structures and Algorithms II</t>
+    <t>Elective 1</t>
+  </si>
+  <si>
+    <t>Elective Subject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -88,6 +91,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,12 +111,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -326,6 +339,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="27.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -360,10 +376,10 @@
       <c r="B2" s="1">
         <v>1.0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="1">
@@ -386,10 +402,10 @@
       <c r="B3" s="1">
         <v>2.0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="1">
@@ -412,10 +428,10 @@
       <c r="B4" s="1">
         <v>1.0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="1">
@@ -433,16 +449,16 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>2025.0</v>
+        <v>2024.0</v>
       </c>
       <c r="B5" s="1">
         <v>2.0</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="E5" s="1">
         <v>10.0</v>

</xml_diff>